<commit_message>
fix lifestage details on group distribution parser and test
</commit_message>
<xml_diff>
--- a/bio_diversity/static/test/parser_test_files/test-indv-distribution.xlsx
+++ b/bio_diversity/static/test/parser_test_files/test-indv-distribution.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>F150</t>
+  </si>
+  <si>
+    <t>Fry</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <dimension ref="A3:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A5:A14"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,13 +714,16 @@
       <c r="R4">
         <v>17</v>
       </c>
+      <c r="S4" t="s">
+        <v>38</v>
+      </c>
       <c r="T4">
         <f t="shared" ref="T4" ca="1" si="0">RANDBETWEEN(250,330) / 10</f>
-        <v>25.3</v>
+        <v>32.9</v>
       </c>
       <c r="U4">
         <f t="shared" ref="U4" ca="1" si="1">RANDBETWEEN(300,400)</f>
-        <v>325</v>
+        <v>396</v>
       </c>
       <c r="V4" t="s">
         <v>34</v>

</xml_diff>